<commit_message>
optimized search and added repo selection script
</commit_message>
<xml_diff>
--- a/wagtail_pattern_verification.xlsx
+++ b/wagtail_pattern_verification.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danarapp/Desktop/scientific-software-architecture-analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danarapp/Desktop/energypattern-keyword-search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41BFBD7-17E9-A448-834F-E0AB3068E9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812DFBD3-0F58-FB4D-82CD-211DA5A2411F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42920" yWindow="-15080" windowWidth="41420" windowHeight="26600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="920" windowWidth="29940" windowHeight="16880" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="git_datatransfer" sheetId="1" r:id="rId1"/>
     <sheet name="comments_datatransfer" sheetId="2" r:id="rId2"/>
-    <sheet name="git_ui" sheetId="3" r:id="rId3"/>
-    <sheet name="comments_ui" sheetId="4" r:id="rId4"/>
+    <sheet name="git_UI" sheetId="3" r:id="rId3"/>
+    <sheet name="comments_UI" sheetId="4" r:id="rId4"/>
     <sheet name="git_code_optimization" sheetId="5" r:id="rId5"/>
     <sheet name="comments_code_optimization" sheetId="6" r:id="rId6"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2245" uniqueCount="614">
   <si>
     <t>row_id</t>
   </si>
@@ -1490,9 +1490,6 @@
   </si>
   <si>
     <t>Make sure that this list is sorted by the codename (first item in the tuple) so that we can follow the same order when querying the Permission objects.</t>
-  </si>
-  <si>
-    <t>commit_link</t>
   </si>
   <si>
     <t>comment</t>
@@ -1942,10 +1939,10 @@
     <t xml:space="preserve">g1_avoid_recompute, cache </t>
   </si>
   <si>
-    <t>https://github.com/wagtail/wagtail/pull/3188/commits/10fb6bd5786fe9db15cc1da414a35f669b29ec1d</t>
-  </si>
-  <si>
     <t>bug fix</t>
+  </si>
+  <si>
+    <t>commit_url</t>
   </si>
 </sst>
 </file>
@@ -2023,7 +2020,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -2046,12 +2043,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2063,6 +2071,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -2368,8 +2379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I143"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2397,10 +2408,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2463,7 +2474,7 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2526,10 +2537,10 @@
         <v>15</v>
       </c>
       <c r="G7" t="s">
+        <v>486</v>
+      </c>
+      <c r="H7" t="s">
         <v>487</v>
-      </c>
-      <c r="H7" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -2572,10 +2583,10 @@
         <v>22</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="H9" t="s">
         <v>489</v>
-      </c>
-      <c r="H9" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -2598,7 +2609,7 @@
         <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2621,7 +2632,7 @@
         <v>22</v>
       </c>
       <c r="H11" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -2724,10 +2735,10 @@
         <v>22</v>
       </c>
       <c r="G16" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="H16" t="s">
         <v>492</v>
-      </c>
-      <c r="H16" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -2830,10 +2841,10 @@
         <v>22</v>
       </c>
       <c r="G21" t="s">
+        <v>493</v>
+      </c>
+      <c r="H21" t="s">
         <v>494</v>
-      </c>
-      <c r="H21" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -2856,7 +2867,7 @@
         <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -2999,7 +3010,7 @@
         <v>10</v>
       </c>
       <c r="H29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -3022,7 +3033,7 @@
         <v>10</v>
       </c>
       <c r="H30" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -3045,7 +3056,7 @@
         <v>10</v>
       </c>
       <c r="H31" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -3068,7 +3079,7 @@
         <v>10</v>
       </c>
       <c r="H32" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -3091,7 +3102,7 @@
         <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -3114,7 +3125,7 @@
         <v>10</v>
       </c>
       <c r="H34" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -3137,7 +3148,7 @@
         <v>10</v>
       </c>
       <c r="H35" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -3160,7 +3171,7 @@
         <v>10</v>
       </c>
       <c r="H36" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -3183,7 +3194,7 @@
         <v>10</v>
       </c>
       <c r="H37" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -3206,7 +3217,7 @@
         <v>10</v>
       </c>
       <c r="H38" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -3229,7 +3240,7 @@
         <v>10</v>
       </c>
       <c r="H39" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -3252,7 +3263,7 @@
         <v>59</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -3275,7 +3286,7 @@
         <v>59</v>
       </c>
       <c r="H41" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -3298,7 +3309,7 @@
         <v>15</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -3321,7 +3332,7 @@
         <v>15</v>
       </c>
       <c r="H43" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -3344,7 +3355,7 @@
         <v>10</v>
       </c>
       <c r="H44" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -3367,7 +3378,7 @@
         <v>10</v>
       </c>
       <c r="H45" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -3390,7 +3401,7 @@
         <v>22</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -3413,7 +3424,7 @@
         <v>22</v>
       </c>
       <c r="H47" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -3436,7 +3447,7 @@
         <v>10</v>
       </c>
       <c r="H48" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -3459,7 +3470,7 @@
         <v>10</v>
       </c>
       <c r="H49" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -3482,7 +3493,7 @@
         <v>15</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -3505,7 +3516,7 @@
         <v>15</v>
       </c>
       <c r="H51" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -3528,10 +3539,10 @@
         <v>76</v>
       </c>
       <c r="G52" t="s">
+        <v>508</v>
+      </c>
+      <c r="H52" t="s">
         <v>509</v>
-      </c>
-      <c r="H52" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -3554,7 +3565,7 @@
         <v>10</v>
       </c>
       <c r="H53" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -3577,7 +3588,7 @@
         <v>10</v>
       </c>
       <c r="H54" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -3600,10 +3611,10 @@
         <v>15</v>
       </c>
       <c r="G55" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="H55" t="s">
         <v>513</v>
-      </c>
-      <c r="H55" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -3626,7 +3637,7 @@
         <v>10</v>
       </c>
       <c r="H56" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -3649,7 +3660,7 @@
         <v>10</v>
       </c>
       <c r="H57" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -3672,7 +3683,7 @@
         <v>10</v>
       </c>
       <c r="H58" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -3695,7 +3706,7 @@
         <v>10</v>
       </c>
       <c r="H59" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -3718,7 +3729,7 @@
         <v>10</v>
       </c>
       <c r="H60" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -3741,7 +3752,7 @@
         <v>10</v>
       </c>
       <c r="H61" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -3764,7 +3775,7 @@
         <v>10</v>
       </c>
       <c r="H62" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -3787,7 +3798,7 @@
         <v>10</v>
       </c>
       <c r="H63" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -3810,7 +3821,7 @@
         <v>10</v>
       </c>
       <c r="H64" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -3833,7 +3844,7 @@
         <v>10</v>
       </c>
       <c r="H65" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -3856,7 +3867,7 @@
         <v>10</v>
       </c>
       <c r="H66" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -3879,7 +3890,7 @@
         <v>10</v>
       </c>
       <c r="H67" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -3902,7 +3913,7 @@
         <v>10</v>
       </c>
       <c r="H68" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -3925,7 +3936,7 @@
         <v>10</v>
       </c>
       <c r="H69" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
@@ -3948,7 +3959,7 @@
         <v>10</v>
       </c>
       <c r="H70" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
@@ -3971,7 +3982,7 @@
         <v>10</v>
       </c>
       <c r="H71" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -3994,10 +4005,10 @@
         <v>15</v>
       </c>
       <c r="G72" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="H72" t="s">
         <v>520</v>
-      </c>
-      <c r="H72" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -4020,7 +4031,7 @@
         <v>10</v>
       </c>
       <c r="H73" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -4043,7 +4054,7 @@
         <v>10</v>
       </c>
       <c r="H74" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
@@ -4066,10 +4077,10 @@
         <v>22</v>
       </c>
       <c r="G75" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="H75" t="s">
         <v>523</v>
-      </c>
-      <c r="H75" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
@@ -4092,7 +4103,7 @@
         <v>10</v>
       </c>
       <c r="H76" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -4115,7 +4126,7 @@
         <v>10</v>
       </c>
       <c r="H77" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -4138,7 +4149,7 @@
         <v>10</v>
       </c>
       <c r="H78" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -4161,7 +4172,7 @@
         <v>10</v>
       </c>
       <c r="H79" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -4184,7 +4195,7 @@
         <v>10</v>
       </c>
       <c r="H80" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -4207,7 +4218,7 @@
         <v>10</v>
       </c>
       <c r="H81" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -4230,7 +4241,7 @@
         <v>10</v>
       </c>
       <c r="H82" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -4253,7 +4264,7 @@
         <v>10</v>
       </c>
       <c r="H83" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -4276,7 +4287,7 @@
         <v>10</v>
       </c>
       <c r="H84" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -4299,7 +4310,7 @@
         <v>10</v>
       </c>
       <c r="H85" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -4322,7 +4333,7 @@
         <v>10</v>
       </c>
       <c r="H86" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -4345,7 +4356,7 @@
         <v>10</v>
       </c>
       <c r="H87" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -4368,7 +4379,7 @@
         <v>10</v>
       </c>
       <c r="H88" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -4391,7 +4402,7 @@
         <v>10</v>
       </c>
       <c r="H89" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -4414,7 +4425,7 @@
         <v>10</v>
       </c>
       <c r="H90" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -4437,7 +4448,7 @@
         <v>10</v>
       </c>
       <c r="H91" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -4460,7 +4471,7 @@
         <v>10</v>
       </c>
       <c r="H92" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -4483,7 +4494,7 @@
         <v>10</v>
       </c>
       <c r="H93" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -4506,7 +4517,7 @@
         <v>10</v>
       </c>
       <c r="H94" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -4530,7 +4541,7 @@
         <v>10</v>
       </c>
       <c r="H95" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -4554,7 +4565,7 @@
         <v>10</v>
       </c>
       <c r="H96" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -4578,7 +4589,7 @@
         <v>10</v>
       </c>
       <c r="H97" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -4602,7 +4613,7 @@
         <v>10</v>
       </c>
       <c r="H98" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
@@ -4623,13 +4634,13 @@
         <v>open</v>
       </c>
       <c r="F99" t="s">
+        <v>542</v>
+      </c>
+      <c r="H99" t="s">
         <v>543</v>
       </c>
-      <c r="H99" t="s">
-        <v>544</v>
-      </c>
       <c r="I99" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
@@ -4653,7 +4664,7 @@
         <v>10</v>
       </c>
       <c r="H100" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -4677,7 +4688,7 @@
         <v>10</v>
       </c>
       <c r="H101" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
@@ -4701,7 +4712,7 @@
         <v>10</v>
       </c>
       <c r="H102" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
@@ -4722,13 +4733,13 @@
         <v>open</v>
       </c>
       <c r="F103" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H103" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I103" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
@@ -4752,7 +4763,7 @@
         <v>10</v>
       </c>
       <c r="H104" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
@@ -4776,7 +4787,7 @@
         <v>10</v>
       </c>
       <c r="H105" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
@@ -4800,7 +4811,7 @@
         <v>10</v>
       </c>
       <c r="H106" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
@@ -4824,7 +4835,7 @@
         <v>10</v>
       </c>
       <c r="H107" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
@@ -4848,7 +4859,7 @@
         <v>10</v>
       </c>
       <c r="H108" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
@@ -4872,7 +4883,7 @@
         <v>10</v>
       </c>
       <c r="H109" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
@@ -4896,7 +4907,7 @@
         <v>10</v>
       </c>
       <c r="H110" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
@@ -4920,7 +4931,7 @@
         <v>10</v>
       </c>
       <c r="H111" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
@@ -4944,7 +4955,7 @@
         <v>10</v>
       </c>
       <c r="H112" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -4968,7 +4979,7 @@
         <v>10</v>
       </c>
       <c r="H113" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -4992,7 +5003,7 @@
         <v>10</v>
       </c>
       <c r="H114" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -5016,7 +5027,7 @@
         <v>10</v>
       </c>
       <c r="H115" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -5040,7 +5051,7 @@
         <v>10</v>
       </c>
       <c r="H116" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -5064,7 +5075,7 @@
         <v>10</v>
       </c>
       <c r="H117" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -5088,7 +5099,7 @@
         <v>10</v>
       </c>
       <c r="H118" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -5112,7 +5123,7 @@
         <v>10</v>
       </c>
       <c r="H119" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -5136,7 +5147,7 @@
         <v>10</v>
       </c>
       <c r="H120" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -5160,7 +5171,7 @@
         <v>10</v>
       </c>
       <c r="H121" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -5292,7 +5303,7 @@
         <v>10</v>
       </c>
       <c r="H128" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -5313,13 +5324,13 @@
         <v>open</v>
       </c>
       <c r="F129" s="8" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H129" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
@@ -5343,7 +5354,7 @@
         <v>10</v>
       </c>
       <c r="H130" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
@@ -5367,7 +5378,7 @@
         <v>10</v>
       </c>
       <c r="H131" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
@@ -5391,7 +5402,7 @@
         <v>10</v>
       </c>
       <c r="H132" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.2">
@@ -5415,7 +5426,7 @@
         <v>10</v>
       </c>
       <c r="H133" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.2">
@@ -5439,7 +5450,7 @@
         <v>10</v>
       </c>
       <c r="H134" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.2">
@@ -5535,7 +5546,7 @@
         <v>10</v>
       </c>
       <c r="H139" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.2">
@@ -5559,7 +5570,7 @@
         <v>10</v>
       </c>
       <c r="H140" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.2">
@@ -5583,7 +5594,7 @@
         <v>10</v>
       </c>
       <c r="H141" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.2">
@@ -5607,7 +5618,7 @@
         <v>10</v>
       </c>
       <c r="H142" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.2">
@@ -5631,7 +5642,7 @@
         <v>10</v>
       </c>
       <c r="H143" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -5649,13 +5660,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5674,8 +5687,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -5695,7 +5714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>7</v>
       </c>
@@ -5724,8 +5743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H262"/>
   <sheetViews>
-    <sheetView topLeftCell="A261" workbookViewId="0">
-      <selection activeCell="I330" sqref="I330"/>
+    <sheetView topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5734,7 +5753,7 @@
     <col min="7" max="7" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5753,8 +5772,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5771,7 +5796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5788,7 +5813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5805,7 +5830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5822,7 +5847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5839,7 +5864,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5856,7 +5881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>8</v>
       </c>
@@ -5873,7 +5898,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>12</v>
       </c>
@@ -5890,7 +5915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>13</v>
       </c>
@@ -5907,7 +5932,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
@@ -5924,7 +5949,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>17</v>
       </c>
@@ -5941,7 +5966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>18</v>
       </c>
@@ -5958,7 +5983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>19</v>
       </c>
@@ -5975,7 +6000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20</v>
       </c>
@@ -5992,7 +6017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>21</v>
       </c>
@@ -9789,7 +9814,7 @@
         <v>10</v>
       </c>
       <c r="H238" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.2">
@@ -9810,10 +9835,10 @@
         <v>open</v>
       </c>
       <c r="F239" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H239" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.2">
@@ -9837,7 +9862,7 @@
         <v>10</v>
       </c>
       <c r="H240" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.2">
@@ -9858,10 +9883,10 @@
         <v>open</v>
       </c>
       <c r="F241" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="H241" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.2">
@@ -9885,7 +9910,7 @@
         <v>10</v>
       </c>
       <c r="H242" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.2">
@@ -9909,7 +9934,7 @@
         <v>10</v>
       </c>
       <c r="H243" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.2">
@@ -9930,13 +9955,13 @@
         <v>open</v>
       </c>
       <c r="F244" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G244" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="H244" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.2">
@@ -9957,10 +9982,10 @@
         <v>open</v>
       </c>
       <c r="F245" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H245" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.2">
@@ -9984,7 +10009,7 @@
         <v>10</v>
       </c>
       <c r="H246" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.2">
@@ -10005,10 +10030,10 @@
         <v>open</v>
       </c>
       <c r="F247" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H247" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.2">
@@ -10029,13 +10054,13 @@
         <v>open</v>
       </c>
       <c r="F248" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G248" t="s">
+        <v>588</v>
+      </c>
+      <c r="H248" t="s">
         <v>589</v>
-      </c>
-      <c r="H248" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.2">
@@ -10056,13 +10081,13 @@
         <v>open</v>
       </c>
       <c r="F249" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G249" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="H249" s="5" t="s">
         <v>587</v>
-      </c>
-      <c r="H249" s="5" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.2">
@@ -10083,10 +10108,10 @@
         <v>open</v>
       </c>
       <c r="F250" t="s">
+        <v>584</v>
+      </c>
+      <c r="H250" t="s">
         <v>585</v>
-      </c>
-      <c r="H250" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.2">
@@ -10107,13 +10132,13 @@
         <v>open</v>
       </c>
       <c r="F251" s="6" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G251" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="H251" s="5" t="s">
         <v>583</v>
-      </c>
-      <c r="H251" s="5" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.2">
@@ -10137,7 +10162,7 @@
         <v>10</v>
       </c>
       <c r="H252" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.2">
@@ -10161,7 +10186,7 @@
         <v>10</v>
       </c>
       <c r="H253" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.2">
@@ -10185,7 +10210,7 @@
         <v>10</v>
       </c>
       <c r="H254" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.2">
@@ -10209,7 +10234,7 @@
         <v>10</v>
       </c>
       <c r="H255" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.2">
@@ -10230,13 +10255,13 @@
         <v>open</v>
       </c>
       <c r="F256" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="G256" t="s">
         <v>577</v>
       </c>
-      <c r="G256" t="s">
+      <c r="H256" s="5" t="s">
         <v>578</v>
-      </c>
-      <c r="H256" s="5" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.2">
@@ -10260,7 +10285,7 @@
         <v>10</v>
       </c>
       <c r="H257" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.2">
@@ -10284,7 +10309,7 @@
         <v>10</v>
       </c>
       <c r="H258" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.2">
@@ -10308,7 +10333,7 @@
         <v>10</v>
       </c>
       <c r="H259" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.2">
@@ -10332,7 +10357,7 @@
         <v>10</v>
       </c>
       <c r="H260" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.2">
@@ -10356,7 +10381,7 @@
         <v>10</v>
       </c>
       <c r="H261" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.2">
@@ -10377,10 +10402,10 @@
         <v>open</v>
       </c>
       <c r="F262" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H262" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -10395,15 +10420,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10422,8 +10447,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G1" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -10441,13 +10472,13 @@
         <v>open</v>
       </c>
       <c r="F2" t="s">
+        <v>600</v>
+      </c>
+      <c r="H2" t="s">
         <v>601</v>
       </c>
-      <c r="I2" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -10467,11 +10498,11 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -10491,11 +10522,11 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -10515,11 +10546,11 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -10539,11 +10570,11 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -10563,11 +10594,11 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="I7" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -10587,11 +10618,11 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="I8" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10611,11 +10642,11 @@
       <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10635,11 +10666,11 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="I10" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10659,11 +10690,11 @@
       <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="I11" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10683,11 +10714,11 @@
       <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="I12" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10707,11 +10738,11 @@
       <c r="F13" t="s">
         <v>10</v>
       </c>
-      <c r="I13" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10731,11 +10762,11 @@
       <c r="F14" t="s">
         <v>10</v>
       </c>
-      <c r="I14" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10755,11 +10786,11 @@
       <c r="F15" t="s">
         <v>10</v>
       </c>
-      <c r="I15" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10779,11 +10810,11 @@
       <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="I16" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10803,11 +10834,11 @@
       <c r="F17" t="s">
         <v>10</v>
       </c>
-      <c r="I17" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10827,11 +10858,11 @@
       <c r="F18" t="s">
         <v>10</v>
       </c>
-      <c r="I18" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10851,11 +10882,11 @@
       <c r="F19" t="s">
         <v>10</v>
       </c>
-      <c r="I19" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10875,11 +10906,11 @@
       <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="I20" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10899,11 +10930,11 @@
       <c r="F21" t="s">
         <v>10</v>
       </c>
-      <c r="I21" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10923,11 +10954,11 @@
       <c r="F22" t="s">
         <v>10</v>
       </c>
-      <c r="I22" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10947,11 +10978,11 @@
       <c r="F23" t="s">
         <v>10</v>
       </c>
-      <c r="I23" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10971,11 +11002,11 @@
       <c r="F24" t="s">
         <v>10</v>
       </c>
-      <c r="I24" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10995,11 +11026,11 @@
       <c r="F25" t="s">
         <v>10</v>
       </c>
-      <c r="I25" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -11019,11 +11050,11 @@
       <c r="F26" t="s">
         <v>10</v>
       </c>
-      <c r="I26" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -11043,11 +11074,11 @@
       <c r="F27" t="s">
         <v>10</v>
       </c>
-      <c r="I27" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
@@ -11067,11 +11098,11 @@
       <c r="F28" t="s">
         <v>10</v>
       </c>
-      <c r="I28" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>29</v>
       </c>
@@ -11091,11 +11122,11 @@
       <c r="F29" t="s">
         <v>10</v>
       </c>
-      <c r="I29" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
@@ -11115,11 +11146,11 @@
       <c r="F30" t="s">
         <v>10</v>
       </c>
-      <c r="I30" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>31</v>
       </c>
@@ -11139,11 +11170,11 @@
       <c r="F31" t="s">
         <v>10</v>
       </c>
-      <c r="I31" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32</v>
       </c>
@@ -11163,11 +11194,11 @@
       <c r="F32" t="s">
         <v>10</v>
       </c>
-      <c r="I32" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
@@ -11187,11 +11218,11 @@
       <c r="F33" t="s">
         <v>10</v>
       </c>
-      <c r="I33" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -11211,8 +11242,8 @@
       <c r="F34" t="s">
         <v>10</v>
       </c>
-      <c r="I34" t="s">
-        <v>594</v>
+      <c r="H34" t="s">
+        <v>593</v>
       </c>
     </row>
   </sheetData>
@@ -11222,15 +11253,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11249,8 +11280,14 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G1" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -11270,11 +11307,11 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="7" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
@@ -11294,11 +11331,11 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>15</v>
       </c>
@@ -11318,11 +11355,11 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>19</v>
       </c>
@@ -11342,11 +11379,11 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20</v>
       </c>
@@ -11366,11 +11403,11 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>26</v>
       </c>
@@ -11390,11 +11427,11 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="I7" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>27</v>
       </c>
@@ -11414,11 +11451,11 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>29</v>
       </c>
@@ -11438,11 +11475,11 @@
       <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="I9" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>34</v>
       </c>
@@ -11462,11 +11499,11 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="I10" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>35</v>
       </c>
@@ -11484,7 +11521,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>36</v>
       </c>
@@ -11502,7 +11539,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>37</v>
       </c>
@@ -11520,7 +11557,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>38</v>
       </c>
@@ -11538,7 +11575,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>41</v>
       </c>
@@ -11556,7 +11593,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>43</v>
       </c>
@@ -11574,7 +11611,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>44</v>
       </c>
@@ -11592,7 +11629,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>45</v>
       </c>
@@ -11610,7 +11647,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>50</v>
       </c>
@@ -11628,7 +11665,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>56</v>
       </c>
@@ -11646,7 +11683,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>57</v>
       </c>
@@ -11664,7 +11701,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>59</v>
       </c>
@@ -11684,11 +11721,11 @@
       <c r="F22" t="s">
         <v>10</v>
       </c>
-      <c r="I22" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>61</v>
       </c>
@@ -11706,7 +11743,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>62</v>
       </c>
@@ -11724,7 +11761,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>69</v>
       </c>
@@ -11742,16 +11779,13 @@
         <v>open</v>
       </c>
       <c r="F25" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="H25" t="s">
-        <v>613</v>
-      </c>
-      <c r="I25" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>70</v>
       </c>
@@ -11769,13 +11803,13 @@
         <v>open</v>
       </c>
       <c r="F26" t="s">
-        <v>612</v>
-      </c>
-      <c r="I26" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+        <v>611</v>
+      </c>
+      <c r="H26" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>71</v>
       </c>
@@ -11793,7 +11827,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>76</v>
       </c>
@@ -11811,7 +11845,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>77</v>
       </c>
@@ -11829,7 +11863,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>78</v>
       </c>
@@ -11847,7 +11881,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>79</v>
       </c>
@@ -11865,7 +11899,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>80</v>
       </c>
@@ -11883,7 +11917,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>83</v>
       </c>
@@ -11901,7 +11935,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>85</v>
       </c>
@@ -11919,7 +11953,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>93</v>
       </c>
@@ -11937,7 +11971,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>94</v>
       </c>
@@ -11955,7 +11989,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>95</v>
       </c>
@@ -11973,7 +12007,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>96</v>
       </c>
@@ -11991,7 +12025,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>99</v>
       </c>
@@ -12009,7 +12043,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>100</v>
       </c>
@@ -12027,7 +12061,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>104</v>
       </c>
@@ -12047,11 +12081,11 @@
       <c r="F41" t="s">
         <v>10</v>
       </c>
-      <c r="I41" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>110</v>
       </c>
@@ -12069,7 +12103,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>112</v>
       </c>
@@ -12087,7 +12121,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>113</v>
       </c>
@@ -12105,7 +12139,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>114</v>
       </c>
@@ -12123,7 +12157,7 @@
         <v>open</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>119</v>
       </c>
@@ -12151,7 +12185,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12175,6 +12209,12 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -12214,7 +12254,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -12238,7 +12278,7 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
   </sheetData>

</xml_diff>